<commit_message>
Rerun test analysis again
</commit_message>
<xml_diff>
--- a/test/cmp/ITS__ITS3-KYO2...ITS4.xlsx
+++ b/test/cmp/ITS__ITS3-KYO2...ITS4.xlsx
@@ -60,10 +60,10 @@
     <t xml:space="preserve">seq17</t>
   </si>
   <si>
+    <t xml:space="preserve">seq8</t>
+  </si>
+  <si>
     <t xml:space="preserve">seq6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seq8</t>
   </si>
   <si>
     <t xml:space="preserve">similar</t>
@@ -484,13 +484,13 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="n">
-        <v>8861</v>
+        <v>8858</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>8862</v>
+        <v>8859</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>1015</v>
+        <v>1728</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>9547</v>
@@ -525,10 +525,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>2283</v>
+        <v>2281</v>
       </c>
       <c r="D3" t="n">
-        <v>2283</v>
+        <v>2281</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -540,10 +540,10 @@
         <v>2372</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>0.25764586389798</v>
+        <v>0.257507337999548</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>0.257616790792146</v>
+        <v>0.257478270685179</v>
       </c>
       <c r="K3" s="2" t="n">
         <v>0</v>
@@ -560,10 +560,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D4" t="n">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="E4" t="n">
         <v>431</v>
@@ -575,13 +575,13 @@
         <v>1560</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>0.170748222548245</v>
+        <v>0.170918943328065</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>0.170728955089145</v>
+        <v>0.170899650073372</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>0.424630541871921</v>
+        <v>0.249421296296296</v>
       </c>
       <c r="L4" s="2" t="n">
         <v>0.16340211584791</v>
@@ -595,13 +595,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
+        <v>1232</v>
+      </c>
+      <c r="D5" t="n">
         <v>1233</v>
       </c>
-      <c r="D5" t="n">
-        <v>1234</v>
-      </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>343</v>
       </c>
       <c r="F5" t="n">
         <v>1268</v>
@@ -610,13 +610,13 @@
         <v>1266</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>0.139149080239251</v>
+        <v>0.13908331451795</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>0.13924621981494</v>
+        <v>0.139180494412462</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>0</v>
+        <v>0.19849537037037</v>
       </c>
       <c r="L5" s="2" t="n">
         <v>0.132816591599455</v>
@@ -630,13 +630,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="D6" t="n">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="F6" t="n">
         <v>1175</v>
@@ -645,13 +645,13 @@
         <v>1175</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>0.128427942670128</v>
+        <v>0.128584330548657</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>0.128413450688332</v>
+        <v>0.128569816006321</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0</v>
+        <v>0.0925925925925926</v>
       </c>
       <c r="L6" s="2" t="n">
         <v>0.123075311616215</v>
@@ -671,7 +671,7 @@
         <v>930</v>
       </c>
       <c r="E7" t="n">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="F7" t="n">
         <v>988</v>
@@ -680,13 +680,13 @@
         <v>988</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>0.104954294097732</v>
+        <v>0.104989839692933</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>0.104942450914015</v>
+        <v>0.104977988486285</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.250246305418719</v>
+        <v>0.149884259259259</v>
       </c>
       <c r="L7" s="2" t="n">
         <v>0.103488006703677</v>
@@ -700,13 +700,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D8" t="n">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E8" t="n">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="F8" t="n">
         <v>942</v>
@@ -715,13 +715,13 @@
         <v>942</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>0.091186096377384</v>
+        <v>0.091104086701287</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>0.0911758068156172</v>
+        <v>0.0910938029122926</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.217733990147783</v>
+        <v>0.129050925925926</v>
       </c>
       <c r="L8" s="2" t="n">
         <v>0.0986697391850843</v>
@@ -741,7 +741,7 @@
         <v>515</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F9" t="n">
         <v>780</v>
@@ -750,13 +750,13 @@
         <v>780</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>0.0581198510326148</v>
+        <v>0.0581395348837209</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>0.0581132927104491</v>
+        <v>0.0581329721187493</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0</v>
+        <v>0.115740740740741</v>
       </c>
       <c r="L9" s="2" t="n">
         <v>0.0817010579239552</v>
@@ -770,10 +770,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D10" t="n">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E10" t="n">
         <v>42</v>
@@ -785,13 +785,13 @@
         <v>165</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>0.0178309445886469</v>
+        <v>0.017724091216979</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>0.0178289325208757</v>
+        <v>0.0177220905294051</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>0.0413793103448276</v>
+        <v>0.0243055555555556</v>
       </c>
       <c r="L10" s="2" t="n">
         <v>0.0172829160992982</v>
@@ -820,13 +820,13 @@
         <v>98</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>0.0107211375691231</v>
+        <v>0.0107247685707835</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>0.0107199277815392</v>
+        <v>0.0107235579636528</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>0.0354679802955665</v>
+        <v>0.0208333333333333</v>
       </c>
       <c r="L11" s="2" t="n">
         <v>0.0102650047135226</v>
@@ -855,10 +855,10 @@
         <v>95</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>0.0106082834894481</v>
+        <v>0.0106118762700384</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>0.0106070864364703</v>
+        <v>0.0106106784061406</v>
       </c>
       <c r="K12" s="2" t="n">
         <v>0</v>
@@ -890,13 +890,13 @@
         <v>40</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>0.00394989278862431</v>
+        <v>0.00395123052607812</v>
       </c>
       <c r="J13" s="2" t="n">
-        <v>0.00394944707740916</v>
+        <v>0.00395078451292471</v>
       </c>
       <c r="K13" s="2" t="n">
-        <v>0.0147783251231527</v>
+        <v>0.00868055555555556</v>
       </c>
       <c r="L13" s="2" t="n">
         <v>0.00418979784225411</v>
@@ -925,10 +925,10 @@
         <v>23</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>0.00259564383252455</v>
+        <v>0.00259652291713705</v>
       </c>
       <c r="J14" s="2" t="n">
-        <v>0.00259535093658316</v>
+        <v>0.00259622982277909</v>
       </c>
       <c r="K14" s="2" t="n">
         <v>0</v>
@@ -960,13 +960,13 @@
         <v>15</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>0.00146710303577474</v>
+        <v>0.00146759990968616</v>
       </c>
       <c r="J15" s="2" t="n">
-        <v>0.00146693748589483</v>
+        <v>0.00146743424765775</v>
       </c>
       <c r="K15" s="2" t="n">
-        <v>0.00689655172413793</v>
+        <v>0.00405092592592593</v>
       </c>
       <c r="L15" s="2" t="n">
         <v>0.00157117419084529</v>
@@ -980,34 +980,34 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D16" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G16" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>0.00124139487642478</v>
+        <v>0.00135470760894107</v>
       </c>
       <c r="J16" s="2" t="n">
-        <v>0.00124125479575717</v>
+        <v>0.00135455469014561</v>
       </c>
       <c r="K16" s="2" t="n">
-        <v>0.00886699507389163</v>
+        <v>0.00231481481481481</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>0.00125693935267623</v>
+        <v>0.00146642924478894</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>0.00125720272393924</v>
+        <v>0.00146673651126244</v>
       </c>
     </row>
     <row r="17">
@@ -1015,34 +1015,34 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
+        <v>11</v>
+      </c>
+      <c r="D17" t="n">
+        <v>11</v>
+      </c>
+      <c r="E17" t="n">
+        <v>8</v>
+      </c>
+      <c r="F17" t="n">
         <v>12</v>
       </c>
-      <c r="D17" t="n">
+      <c r="G17" t="n">
         <v>12</v>
       </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>14</v>
-      </c>
-      <c r="G17" t="n">
-        <v>14</v>
-      </c>
       <c r="I17" s="2" t="n">
-        <v>0.00135424895609976</v>
+        <v>0.00124181530819598</v>
       </c>
       <c r="J17" s="2" t="n">
-        <v>0.001354096140826</v>
+        <v>0.00124167513263348</v>
       </c>
       <c r="K17" s="2" t="n">
-        <v>0</v>
+        <v>0.00462962962962963</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>0.00146642924478894</v>
+        <v>0.00125693935267623</v>
       </c>
       <c r="M17" s="2" t="n">
-        <v>0.00146673651126244</v>
+        <v>0.00125720272393924</v>
       </c>
     </row>
   </sheetData>
@@ -1133,13 +1133,13 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="n">
-        <v>4636</v>
+        <v>4633</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>4628</v>
+        <v>4625</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>760</v>
+        <v>876</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>4892</v>
@@ -1174,13 +1174,13 @@
         <v>23</v>
       </c>
       <c r="C3" t="n">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="D3" t="n">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="E3" t="n">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="F3" t="n">
         <v>2108</v>
@@ -1189,13 +1189,13 @@
         <v>2108</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>0.422993960310613</v>
+        <v>0.423052018130801</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>0.423725151253241</v>
+        <v>0.423783783783784</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>0.776315789473684</v>
+        <v>0.674657534246575</v>
       </c>
       <c r="L3" s="2" t="n">
         <v>0.43090760425184</v>
@@ -1209,10 +1209,10 @@
         <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>1495</v>
+        <v>1492</v>
       </c>
       <c r="D4" t="n">
-        <v>1495</v>
+        <v>1492</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -1224,10 +1224,10 @@
         <v>1568</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>0.322476272648835</v>
+        <v>0.322037556658752</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>0.323033707865169</v>
+        <v>0.322594594594595</v>
       </c>
       <c r="K4" s="2" t="n">
         <v>0</v>
@@ -1241,7 +1241,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" t="n">
         <v>615</v>
@@ -1250,7 +1250,7 @@
         <v>615</v>
       </c>
       <c r="E5" t="n">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F5" t="n">
         <v>637</v>
@@ -1259,13 +1259,13 @@
         <v>637</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>0.132657463330457</v>
+        <v>0.132743362831858</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>0.132886776145203</v>
+        <v>0.132972972972973</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>0.209210526315789</v>
+        <v>0.182648401826484</v>
       </c>
       <c r="L5" s="2" t="n">
         <v>0.130212591986917</v>
@@ -1276,7 +1276,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="n">
         <v>176</v>
@@ -1285,7 +1285,7 @@
         <v>176</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="F6" t="n">
         <v>182</v>
@@ -1294,13 +1294,13 @@
         <v>182</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>0.0379637618636756</v>
+        <v>0.0379883444852148</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>0.0380293863439931</v>
+        <v>0.0380540540540541</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0</v>
+        <v>0.0593607305936073</v>
       </c>
       <c r="L6" s="2" t="n">
         <v>0.0372035977105478</v>
@@ -1314,13 +1314,13 @@
         <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D7" t="n">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="F7" t="n">
         <v>169</v>
@@ -1329,13 +1329,13 @@
         <v>169</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>0.0349439171699741</v>
+        <v>0.0351823872221023</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>0.0350043215211755</v>
+        <v>0.0352432432432432</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0</v>
+        <v>0.0490867579908676</v>
       </c>
       <c r="L7" s="2" t="n">
         <v>0.0345461978740801</v>
@@ -1355,7 +1355,7 @@
         <v>134</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F8" t="n">
         <v>138</v>
@@ -1364,13 +1364,13 @@
         <v>138</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>0.0289042277825712</v>
+        <v>0.0289229440966976</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>0.0289541918755402</v>
+        <v>0.028972972972973</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0</v>
+        <v>0.0182648401826484</v>
       </c>
       <c r="L8" s="2" t="n">
         <v>0.0282093213409648</v>
@@ -1399,13 +1399,13 @@
         <v>48</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>0.0103537532355479</v>
+        <v>0.0103604575868768</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>0.010371650821089</v>
+        <v>0.0103783783783784</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.00526315789473684</v>
+        <v>0.0045662100456621</v>
       </c>
       <c r="L9" s="2" t="n">
         <v>0.0098119378577269</v>
@@ -1434,13 +1434,13 @@
         <v>27</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>0.0049611734253667</v>
+        <v>0.00496438592704511</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>0.00496974935177182</v>
+        <v>0.00497297297297297</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>0.00921052631578947</v>
+        <v>0.00799086757990868</v>
       </c>
       <c r="L10" s="2" t="n">
         <v>0.00551921504497138</v>
@@ -1460,7 +1460,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>15</v>
@@ -1469,13 +1469,13 @@
         <v>15</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>0.00301984469370147</v>
+        <v>0.00302180012950572</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>0.00302506482281763</v>
+        <v>0.00302702702702703</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>0</v>
+        <v>0.00342465753424658</v>
       </c>
       <c r="L11" s="2" t="n">
         <v>0.00306623058053966</v>
@@ -1504,7 +1504,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>0.00172562553925798</v>
+        <v>0.00172674293114613</v>
       </c>
       <c r="J12" s="2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Restore earlier ITSx default and re-generate output files
</commit_message>
<xml_diff>
--- a/test/cmp/ITS__ITS3-KYO2...ITS4.xlsx
+++ b/test/cmp/ITS__ITS3-KYO2...ITS4.xlsx
@@ -484,13 +484,13 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="n">
-        <v>8858</v>
+        <v>8864</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>8859</v>
+        <v>8865</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>1728</v>
+        <v>1726</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>9547</v>
@@ -525,10 +525,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>2281</v>
+        <v>2283</v>
       </c>
       <c r="D3" t="n">
-        <v>2281</v>
+        <v>2283</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -540,10 +540,10 @@
         <v>2372</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>0.257507337999548</v>
+        <v>0.257558664259928</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>0.257478270685179</v>
+        <v>0.257529610829103</v>
       </c>
       <c r="K3" s="2" t="n">
         <v>0</v>
@@ -575,13 +575,13 @@
         <v>1560</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>0.170918943328065</v>
+        <v>0.170803249097473</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>0.170899650073372</v>
+        <v>0.170783981951495</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>0.249421296296296</v>
+        <v>0.249710312862109</v>
       </c>
       <c r="L4" s="2" t="n">
         <v>0.16340211584791</v>
@@ -595,10 +595,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D5" t="n">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="E5" t="n">
         <v>343</v>
@@ -610,13 +610,13 @@
         <v>1266</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>0.13908331451795</v>
+        <v>0.139101985559567</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>0.139180494412462</v>
+        <v>0.139199097574732</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>0.19849537037037</v>
+        <v>0.198725376593279</v>
       </c>
       <c r="L5" s="2" t="n">
         <v>0.132816591599455</v>
@@ -645,13 +645,13 @@
         <v>1175</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>0.128584330548657</v>
+        <v>0.128497292418773</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>0.128569816006321</v>
+        <v>0.128482797518331</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.0925925925925926</v>
+        <v>0.0926998841251448</v>
       </c>
       <c r="L6" s="2" t="n">
         <v>0.123075311616215</v>
@@ -665,13 +665,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="D7" t="n">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="E7" t="n">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F7" t="n">
         <v>988</v>
@@ -680,13 +680,13 @@
         <v>988</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>0.104989839692933</v>
+        <v>0.105031588447653</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>0.104977988486285</v>
+        <v>0.105019740552735</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.149884259259259</v>
+        <v>0.149478563151796</v>
       </c>
       <c r="L7" s="2" t="n">
         <v>0.103488006703677</v>
@@ -700,10 +700,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="D8" t="n">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="E8" t="n">
         <v>223</v>
@@ -715,13 +715,13 @@
         <v>942</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>0.091104086701287</v>
+        <v>0.0911552346570397</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>0.0910938029122926</v>
+        <v>0.0911449520586576</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.129050925925926</v>
+        <v>0.129200463499421</v>
       </c>
       <c r="L8" s="2" t="n">
         <v>0.0986697391850843</v>
@@ -741,7 +741,7 @@
         <v>515</v>
       </c>
       <c r="E9" t="n">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F9" t="n">
         <v>780</v>
@@ -750,13 +750,13 @@
         <v>780</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>0.0581395348837209</v>
+        <v>0.0581001805054152</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>0.0581329721187493</v>
+        <v>0.0580936266215454</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.115740740740741</v>
+        <v>0.115295480880649</v>
       </c>
       <c r="L9" s="2" t="n">
         <v>0.0817010579239552</v>
@@ -770,10 +770,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D10" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E10" t="n">
         <v>42</v>
@@ -785,13 +785,13 @@
         <v>165</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>0.017724091216979</v>
+        <v>0.0178249097472924</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>0.0177220905294051</v>
+        <v>0.0178228990411732</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>0.0243055555555556</v>
+        <v>0.0243337195828505</v>
       </c>
       <c r="L10" s="2" t="n">
         <v>0.0172829160992982</v>
@@ -820,13 +820,13 @@
         <v>98</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>0.0107247685707835</v>
+        <v>0.0107175090252708</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>0.0107235579636528</v>
+        <v>0.0107163000564016</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>0.0208333333333333</v>
+        <v>0.0208574739281576</v>
       </c>
       <c r="L11" s="2" t="n">
         <v>0.0102650047135226</v>
@@ -855,10 +855,10 @@
         <v>95</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>0.0106118762700384</v>
+        <v>0.0106046931407942</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>0.0106106784061406</v>
+        <v>0.0106034968979131</v>
       </c>
       <c r="K12" s="2" t="n">
         <v>0</v>
@@ -890,13 +890,13 @@
         <v>40</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>0.00395123052607812</v>
+        <v>0.0039485559566787</v>
       </c>
       <c r="J13" s="2" t="n">
-        <v>0.00395078451292471</v>
+        <v>0.00394811054709532</v>
       </c>
       <c r="K13" s="2" t="n">
-        <v>0.00868055555555556</v>
+        <v>0.00869061413673233</v>
       </c>
       <c r="L13" s="2" t="n">
         <v>0.00418979784225411</v>
@@ -925,10 +925,10 @@
         <v>23</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>0.00259652291713705</v>
+        <v>0.00259476534296029</v>
       </c>
       <c r="J14" s="2" t="n">
-        <v>0.00259622982277909</v>
+        <v>0.00259447264523407</v>
       </c>
       <c r="K14" s="2" t="n">
         <v>0</v>
@@ -960,13 +960,13 @@
         <v>15</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>0.00146759990968616</v>
+        <v>0.00146660649819495</v>
       </c>
       <c r="J15" s="2" t="n">
-        <v>0.00146743424765775</v>
+        <v>0.00146644106034969</v>
       </c>
       <c r="K15" s="2" t="n">
-        <v>0.00405092592592593</v>
+        <v>0.00405561993047509</v>
       </c>
       <c r="L15" s="2" t="n">
         <v>0.00157117419084529</v>
@@ -995,13 +995,13 @@
         <v>14</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>0.00135470760894107</v>
+        <v>0.00135379061371841</v>
       </c>
       <c r="J16" s="2" t="n">
-        <v>0.00135455469014561</v>
+        <v>0.00135363790186125</v>
       </c>
       <c r="K16" s="2" t="n">
-        <v>0.00231481481481481</v>
+        <v>0.00231749710312862</v>
       </c>
       <c r="L16" s="2" t="n">
         <v>0.00146642924478894</v>
@@ -1030,13 +1030,13 @@
         <v>12</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>0.00124181530819598</v>
+        <v>0.00124097472924188</v>
       </c>
       <c r="J17" s="2" t="n">
-        <v>0.00124167513263348</v>
+        <v>0.00124083474337281</v>
       </c>
       <c r="K17" s="2" t="n">
-        <v>0.00462962962962963</v>
+        <v>0.00463499420625724</v>
       </c>
       <c r="L17" s="2" t="n">
         <v>0.00125693935267623</v>
@@ -1133,13 +1133,13 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="n">
-        <v>4633</v>
+        <v>4638</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>4625</v>
+        <v>4630</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>4892</v>
@@ -1174,10 +1174,10 @@
         <v>23</v>
       </c>
       <c r="C3" t="n">
-        <v>1960</v>
+        <v>1961</v>
       </c>
       <c r="D3" t="n">
-        <v>1960</v>
+        <v>1961</v>
       </c>
       <c r="E3" t="n">
         <v>591</v>
@@ -1189,13 +1189,13 @@
         <v>2108</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>0.423052018130801</v>
+        <v>0.422811556705476</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>0.423783783783784</v>
+        <v>0.42354211663067</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>0.674657534246575</v>
+        <v>0.673888255416192</v>
       </c>
       <c r="L3" s="2" t="n">
         <v>0.43090760425184</v>
@@ -1209,10 +1209,10 @@
         <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>1492</v>
+        <v>1494</v>
       </c>
       <c r="D4" t="n">
-        <v>1492</v>
+        <v>1494</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -1224,10 +1224,10 @@
         <v>1568</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>0.322037556658752</v>
+        <v>0.322121604139715</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>0.322594594594595</v>
+        <v>0.32267818574514</v>
       </c>
       <c r="K4" s="2" t="n">
         <v>0</v>
@@ -1244,10 +1244,10 @@
         <v>16</v>
       </c>
       <c r="C5" t="n">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="D5" t="n">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="E5" t="n">
         <v>160</v>
@@ -1259,13 +1259,13 @@
         <v>637</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>0.132743362831858</v>
+        <v>0.133031479085813</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>0.132972972972973</v>
+        <v>0.133261339092873</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>0.182648401826484</v>
+        <v>0.182440136830103</v>
       </c>
       <c r="L5" s="2" t="n">
         <v>0.130212591986917</v>
@@ -1294,13 +1294,13 @@
         <v>182</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>0.0379883444852148</v>
+        <v>0.0379473911168607</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>0.0380540540540541</v>
+        <v>0.0380129589632829</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.0593607305936073</v>
+        <v>0.0592930444697834</v>
       </c>
       <c r="L6" s="2" t="n">
         <v>0.0372035977105478</v>
@@ -1320,7 +1320,7 @@
         <v>163</v>
       </c>
       <c r="E7" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F7" t="n">
         <v>169</v>
@@ -1329,13 +1329,13 @@
         <v>169</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>0.0351823872221023</v>
+        <v>0.0351444588184562</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>0.0352432432432432</v>
+        <v>0.0352051835853132</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.0490867579908676</v>
+        <v>0.0501710376282782</v>
       </c>
       <c r="L7" s="2" t="n">
         <v>0.0345461978740801</v>
@@ -1364,13 +1364,13 @@
         <v>138</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>0.0289229440966976</v>
+        <v>0.0288917636912462</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>0.028972972972973</v>
+        <v>0.0289416846652268</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.0182648401826484</v>
+        <v>0.0182440136830103</v>
       </c>
       <c r="L8" s="2" t="n">
         <v>0.0282093213409648</v>
@@ -1399,13 +1399,13 @@
         <v>48</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>0.0103604575868768</v>
+        <v>0.0103492884864166</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>0.0103783783783784</v>
+        <v>0.0103671706263499</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.0045662100456621</v>
+        <v>0.00456100342075257</v>
       </c>
       <c r="L9" s="2" t="n">
         <v>0.0098119378577269</v>
@@ -1434,13 +1434,13 @@
         <v>27</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>0.00496438592704511</v>
+        <v>0.00495903406640793</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>0.00497297297297297</v>
+        <v>0.00496760259179266</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>0.00799086757990868</v>
+        <v>0.00798175598631699</v>
       </c>
       <c r="L10" s="2" t="n">
         <v>0.00551921504497138</v>
@@ -1469,13 +1469,13 @@
         <v>15</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>0.00302180012950572</v>
+        <v>0.00301854247520483</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>0.00302702702702703</v>
+        <v>0.00302375809935205</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>0.00342465753424658</v>
+        <v>0.00342075256556442</v>
       </c>
       <c r="L11" s="2" t="n">
         <v>0.00306623058053966</v>
@@ -1504,7 +1504,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>0.00172674293114613</v>
+        <v>0.00172488141440276</v>
       </c>
       <c r="J12" s="2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Improve DADA2 option handling, rerun test analysis
* some options renamed
* The option for read filteirng in Amptk DADA2  was not ideal,
   this has been changed.
</commit_message>
<xml_diff>
--- a/test/cmp/ITS__ITS3-KYO2...ITS4.xlsx
+++ b/test/cmp/ITS__ITS3-KYO2...ITS4.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve">sample</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t xml:space="preserve">unoise_usearch_simple paired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unoise_usearch_simple2 paired</t>
   </si>
   <si>
     <t xml:space="preserve">unoise_vsearch_simple paired</t>
@@ -480,29 +483,35 @@
       <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2">
@@ -511,10 +520,10 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="n">
-        <v>8860</v>
+        <v>8858</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>8861</v>
+        <v>8859</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1728</v>
@@ -532,12 +541,12 @@
         <v>9622</v>
       </c>
       <c r="J2" s="1" t="n">
+        <v>9622</v>
+      </c>
+      <c r="K2" s="1" t="n">
         <v>9371</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="L2" s="1"/>
       <c r="M2" s="1" t="n">
         <v>1</v>
       </c>
@@ -559,14 +568,21 @@
       <c r="S2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
+      <c r="T2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -594,22 +610,22 @@
         <v>2388</v>
       </c>
       <c r="J3" t="n">
+        <v>2388</v>
+      </c>
+      <c r="K3" t="n">
         <v>2366</v>
       </c>
-      <c r="L3" s="2" t="n">
-        <v>0.25744920993228</v>
-      </c>
       <c r="M3" s="2" t="n">
-        <v>0.25742015573863</v>
+        <v>0.257507337999548</v>
       </c>
       <c r="N3" s="2" t="n">
-        <v>0</v>
+        <v>0.257478270685179</v>
       </c>
       <c r="O3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2" t="n">
         <v>0.252481058584996</v>
-      </c>
-      <c r="P3" s="2" t="n">
-        <v>0.248181251299106</v>
       </c>
       <c r="Q3" s="2" t="n">
         <v>0.248181251299106</v>
@@ -618,6 +634,12 @@
         <v>0.248181251299106</v>
       </c>
       <c r="S3" s="2" t="n">
+        <v>0.248181251299106</v>
+      </c>
+      <c r="T3" s="2" t="n">
+        <v>0.248181251299106</v>
+      </c>
+      <c r="U3" s="2" t="n">
         <v>0.252481058584996</v>
       </c>
     </row>
@@ -626,10 +648,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="D4" t="n">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="E4" t="n">
         <v>431</v>
@@ -647,22 +669,22 @@
         <v>1570</v>
       </c>
       <c r="J4" t="n">
+        <v>1570</v>
+      </c>
+      <c r="K4" t="n">
         <v>1561</v>
       </c>
-      <c r="L4" s="2" t="n">
-        <v>0.170993227990971</v>
-      </c>
       <c r="M4" s="2" t="n">
-        <v>0.170973930707595</v>
+        <v>0.170918943328065</v>
       </c>
       <c r="N4" s="2" t="n">
+        <v>0.170899650073372</v>
+      </c>
+      <c r="O4" s="2" t="n">
         <v>0.249421296296296</v>
       </c>
-      <c r="O4" s="2" t="n">
+      <c r="P4" s="2" t="n">
         <v>0.166577739835663</v>
-      </c>
-      <c r="P4" s="2" t="n">
-        <v>0.163167740594471</v>
       </c>
       <c r="Q4" s="2" t="n">
         <v>0.163167740594471</v>
@@ -671,6 +693,12 @@
         <v>0.163167740594471</v>
       </c>
       <c r="S4" s="2" t="n">
+        <v>0.163167740594471</v>
+      </c>
+      <c r="T4" s="2" t="n">
+        <v>0.163167740594471</v>
+      </c>
+      <c r="U4" s="2" t="n">
         <v>0.166577739835663</v>
       </c>
     </row>
@@ -700,22 +728,22 @@
         <v>1282</v>
       </c>
       <c r="J5" t="n">
+        <v>1282</v>
+      </c>
+      <c r="K5" t="n">
         <v>1276</v>
       </c>
-      <c r="L5" s="2" t="n">
-        <v>0.139051918735892</v>
-      </c>
       <c r="M5" s="2" t="n">
-        <v>0.139149080239251</v>
+        <v>0.13908331451795</v>
       </c>
       <c r="N5" s="2" t="n">
+        <v>0.139180494412462</v>
+      </c>
+      <c r="O5" s="2" t="n">
         <v>0.19849537037037</v>
       </c>
-      <c r="O5" s="2" t="n">
+      <c r="P5" s="2" t="n">
         <v>0.136164763632483</v>
-      </c>
-      <c r="P5" s="2" t="n">
-        <v>0.133236333402619</v>
       </c>
       <c r="Q5" s="2" t="n">
         <v>0.133236333402619</v>
@@ -724,6 +752,12 @@
         <v>0.133236333402619</v>
       </c>
       <c r="S5" s="2" t="n">
+        <v>0.133236333402619</v>
+      </c>
+      <c r="T5" s="2" t="n">
+        <v>0.133236333402619</v>
+      </c>
+      <c r="U5" s="2" t="n">
         <v>0.136164763632483</v>
       </c>
     </row>
@@ -753,22 +787,22 @@
         <v>1184</v>
       </c>
       <c r="J6" t="n">
+        <v>1184</v>
+      </c>
+      <c r="K6" t="n">
         <v>1177</v>
       </c>
-      <c r="L6" s="2" t="n">
-        <v>0.128555304740406</v>
-      </c>
       <c r="M6" s="2" t="n">
-        <v>0.128540796749803</v>
+        <v>0.128584330548657</v>
       </c>
       <c r="N6" s="2" t="n">
+        <v>0.128569816006321</v>
+      </c>
+      <c r="O6" s="2" t="n">
         <v>0.0925925925925926</v>
       </c>
-      <c r="O6" s="2" t="n">
+      <c r="P6" s="2" t="n">
         <v>0.125600256109273</v>
-      </c>
-      <c r="P6" s="2" t="n">
-        <v>0.123051340677614</v>
       </c>
       <c r="Q6" s="2" t="n">
         <v>0.123051340677614</v>
@@ -777,6 +811,12 @@
         <v>0.123051340677614</v>
       </c>
       <c r="S6" s="2" t="n">
+        <v>0.123051340677614</v>
+      </c>
+      <c r="T6" s="2" t="n">
+        <v>0.123051340677614</v>
+      </c>
+      <c r="U6" s="2" t="n">
         <v>0.125600256109273</v>
       </c>
     </row>
@@ -785,10 +825,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="D7" t="n">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E7" t="n">
         <v>259</v>
@@ -806,22 +846,22 @@
         <v>992</v>
       </c>
       <c r="J7" t="n">
+        <v>992</v>
+      </c>
+      <c r="K7" t="n">
         <v>979</v>
       </c>
-      <c r="L7" s="2" t="n">
-        <v>0.105079006772009</v>
-      </c>
       <c r="M7" s="2" t="n">
-        <v>0.105067148177407</v>
+        <v>0.104989839692933</v>
       </c>
       <c r="N7" s="2" t="n">
+        <v>0.104977988486285</v>
+      </c>
+      <c r="O7" s="2" t="n">
         <v>0.149884259259259</v>
       </c>
-      <c r="O7" s="2" t="n">
+      <c r="P7" s="2" t="n">
         <v>0.104471241062853</v>
-      </c>
-      <c r="P7" s="2" t="n">
-        <v>0.103097069216379</v>
       </c>
       <c r="Q7" s="2" t="n">
         <v>0.103097069216379</v>
@@ -830,6 +870,12 @@
         <v>0.103097069216379</v>
       </c>
       <c r="S7" s="2" t="n">
+        <v>0.103097069216379</v>
+      </c>
+      <c r="T7" s="2" t="n">
+        <v>0.103097069216379</v>
+      </c>
+      <c r="U7" s="2" t="n">
         <v>0.104471241062853</v>
       </c>
     </row>
@@ -859,22 +905,22 @@
         <v>946</v>
       </c>
       <c r="J8" t="n">
+        <v>946</v>
+      </c>
+      <c r="K8" t="n">
         <v>929</v>
       </c>
-      <c r="L8" s="2" t="n">
-        <v>0.0910835214446953</v>
-      </c>
       <c r="M8" s="2" t="n">
-        <v>0.0910732422977091</v>
+        <v>0.091104086701287</v>
       </c>
       <c r="N8" s="2" t="n">
+        <v>0.0910938029122926</v>
+      </c>
+      <c r="O8" s="2" t="n">
         <v>0.129050925925926</v>
       </c>
-      <c r="O8" s="2" t="n">
+      <c r="P8" s="2" t="n">
         <v>0.0991356312026465</v>
-      </c>
-      <c r="P8" s="2" t="n">
-        <v>0.0983163583454583</v>
       </c>
       <c r="Q8" s="2" t="n">
         <v>0.0983163583454583</v>
@@ -883,6 +929,12 @@
         <v>0.0983163583454583</v>
       </c>
       <c r="S8" s="2" t="n">
+        <v>0.0983163583454583</v>
+      </c>
+      <c r="T8" s="2" t="n">
+        <v>0.0983163583454583</v>
+      </c>
+      <c r="U8" s="2" t="n">
         <v>0.0991356312026465</v>
       </c>
     </row>
@@ -912,22 +964,22 @@
         <v>789</v>
       </c>
       <c r="J9" t="n">
+        <v>789</v>
+      </c>
+      <c r="K9" t="n">
         <v>621</v>
       </c>
-      <c r="L9" s="2" t="n">
-        <v>0.0581264108352144</v>
-      </c>
       <c r="M9" s="2" t="n">
-        <v>0.0581198510326148</v>
+        <v>0.0581395348837209</v>
       </c>
       <c r="N9" s="2" t="n">
+        <v>0.0581329721187493</v>
+      </c>
+      <c r="O9" s="2" t="n">
         <v>0.115740740740741</v>
       </c>
-      <c r="O9" s="2" t="n">
+      <c r="P9" s="2" t="n">
         <v>0.0662682744637712</v>
-      </c>
-      <c r="P9" s="2" t="n">
-        <v>0.0819995842860112</v>
       </c>
       <c r="Q9" s="2" t="n">
         <v>0.0819995842860112</v>
@@ -936,6 +988,12 @@
         <v>0.0819995842860112</v>
       </c>
       <c r="S9" s="2" t="n">
+        <v>0.0819995842860112</v>
+      </c>
+      <c r="T9" s="2" t="n">
+        <v>0.0819995842860112</v>
+      </c>
+      <c r="U9" s="2" t="n">
         <v>0.0662682744637712</v>
       </c>
     </row>
@@ -965,22 +1023,22 @@
         <v>168</v>
       </c>
       <c r="J10" t="n">
+        <v>168</v>
+      </c>
+      <c r="K10" t="n">
         <v>166</v>
       </c>
-      <c r="L10" s="2" t="n">
-        <v>0.0177200902934537</v>
-      </c>
       <c r="M10" s="2" t="n">
-        <v>0.0177180905089719</v>
+        <v>0.017724091216979</v>
       </c>
       <c r="N10" s="2" t="n">
+        <v>0.0177220905294051</v>
+      </c>
+      <c r="O10" s="2" t="n">
         <v>0.0243055555555556</v>
       </c>
-      <c r="O10" s="2" t="n">
+      <c r="P10" s="2" t="n">
         <v>0.0177142247358873</v>
-      </c>
-      <c r="P10" s="2" t="n">
-        <v>0.0174599875285803</v>
       </c>
       <c r="Q10" s="2" t="n">
         <v>0.0174599875285803</v>
@@ -989,6 +1047,12 @@
         <v>0.0174599875285803</v>
       </c>
       <c r="S10" s="2" t="n">
+        <v>0.0174599875285803</v>
+      </c>
+      <c r="T10" s="2" t="n">
+        <v>0.0174599875285803</v>
+      </c>
+      <c r="U10" s="2" t="n">
         <v>0.0177142247358873</v>
       </c>
     </row>
@@ -1018,22 +1082,22 @@
         <v>99</v>
       </c>
       <c r="J11" t="n">
+        <v>99</v>
+      </c>
+      <c r="K11" t="n">
         <v>98</v>
       </c>
-      <c r="L11" s="2" t="n">
-        <v>0.0107223476297968</v>
-      </c>
       <c r="M11" s="2" t="n">
-        <v>0.0107211375691231</v>
+        <v>0.0107247685707835</v>
       </c>
       <c r="N11" s="2" t="n">
+        <v>0.0107235579636528</v>
+      </c>
+      <c r="O11" s="2" t="n">
         <v>0.0208333333333333</v>
       </c>
-      <c r="O11" s="2" t="n">
+      <c r="P11" s="2" t="n">
         <v>0.0104577953260058</v>
-      </c>
-      <c r="P11" s="2" t="n">
-        <v>0.0102889212221991</v>
       </c>
       <c r="Q11" s="2" t="n">
         <v>0.0102889212221991</v>
@@ -1042,6 +1106,12 @@
         <v>0.0102889212221991</v>
       </c>
       <c r="S11" s="2" t="n">
+        <v>0.0102889212221991</v>
+      </c>
+      <c r="T11" s="2" t="n">
+        <v>0.0102889212221991</v>
+      </c>
+      <c r="U11" s="2" t="n">
         <v>0.0104577953260058</v>
       </c>
     </row>
@@ -1071,22 +1141,22 @@
         <v>97</v>
       </c>
       <c r="J12" t="n">
+        <v>97</v>
+      </c>
+      <c r="K12" t="n">
         <v>95</v>
       </c>
-      <c r="L12" s="2" t="n">
-        <v>0.0106094808126411</v>
-      </c>
       <c r="M12" s="2" t="n">
-        <v>0.0106082834894481</v>
+        <v>0.0106118762700384</v>
       </c>
       <c r="N12" s="2" t="n">
-        <v>0</v>
+        <v>0.0106106784061406</v>
       </c>
       <c r="O12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2" t="n">
         <v>0.0101376587343933</v>
-      </c>
-      <c r="P12" s="2" t="n">
-        <v>0.0100810642278113</v>
       </c>
       <c r="Q12" s="2" t="n">
         <v>0.0100810642278113</v>
@@ -1095,6 +1165,12 @@
         <v>0.0100810642278113</v>
       </c>
       <c r="S12" s="2" t="n">
+        <v>0.0100810642278113</v>
+      </c>
+      <c r="T12" s="2" t="n">
+        <v>0.0100810642278113</v>
+      </c>
+      <c r="U12" s="2" t="n">
         <v>0.0101376587343933</v>
       </c>
     </row>
@@ -1124,22 +1200,22 @@
         <v>41</v>
       </c>
       <c r="J13" t="n">
+        <v>41</v>
+      </c>
+      <c r="K13" t="n">
         <v>38</v>
       </c>
-      <c r="L13" s="2" t="n">
-        <v>0.00395033860045147</v>
-      </c>
       <c r="M13" s="2" t="n">
-        <v>0.00394989278862431</v>
+        <v>0.00395123052607812</v>
       </c>
       <c r="N13" s="2" t="n">
+        <v>0.00395078451292471</v>
+      </c>
+      <c r="O13" s="2" t="n">
         <v>0.00868055555555556</v>
       </c>
-      <c r="O13" s="2" t="n">
+      <c r="P13" s="2" t="n">
         <v>0.00405506349375734</v>
-      </c>
-      <c r="P13" s="2" t="n">
-        <v>0.00426106838495115</v>
       </c>
       <c r="Q13" s="2" t="n">
         <v>0.00426106838495115</v>
@@ -1148,6 +1224,12 @@
         <v>0.00426106838495115</v>
       </c>
       <c r="S13" s="2" t="n">
+        <v>0.00426106838495115</v>
+      </c>
+      <c r="T13" s="2" t="n">
+        <v>0.00426106838495115</v>
+      </c>
+      <c r="U13" s="2" t="n">
         <v>0.00405506349375734</v>
       </c>
     </row>
@@ -1179,20 +1261,20 @@
       <c r="J14" t="n">
         <v>24</v>
       </c>
-      <c r="L14" s="2" t="n">
-        <v>0.00259593679458239</v>
+      <c r="K14" t="n">
+        <v>24</v>
       </c>
       <c r="M14" s="2" t="n">
-        <v>0.00259564383252455</v>
+        <v>0.00259652291713705</v>
       </c>
       <c r="N14" s="2" t="n">
-        <v>0</v>
+        <v>0.00259622982277909</v>
       </c>
       <c r="O14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2" t="n">
         <v>0.00256109273289937</v>
-      </c>
-      <c r="P14" s="2" t="n">
-        <v>0.00249428393265433</v>
       </c>
       <c r="Q14" s="2" t="n">
         <v>0.00249428393265433</v>
@@ -1201,6 +1283,12 @@
         <v>0.00249428393265433</v>
       </c>
       <c r="S14" s="2" t="n">
+        <v>0.00249428393265433</v>
+      </c>
+      <c r="T14" s="2" t="n">
+        <v>0.00249428393265433</v>
+      </c>
+      <c r="U14" s="2" t="n">
         <v>0.00256109273289937</v>
       </c>
     </row>
@@ -1232,20 +1320,20 @@
       <c r="J15" t="n">
         <v>15</v>
       </c>
-      <c r="L15" s="2" t="n">
-        <v>0.00146726862302483</v>
+      <c r="K15" t="n">
+        <v>15</v>
       </c>
       <c r="M15" s="2" t="n">
-        <v>0.00146710303577474</v>
+        <v>0.00146759990968616</v>
       </c>
       <c r="N15" s="2" t="n">
+        <v>0.00146743424765775</v>
+      </c>
+      <c r="O15" s="2" t="n">
         <v>0.00405092592592593</v>
       </c>
-      <c r="O15" s="2" t="n">
+      <c r="P15" s="2" t="n">
         <v>0.00160068295806211</v>
-      </c>
-      <c r="P15" s="2" t="n">
-        <v>0.00155892745790896</v>
       </c>
       <c r="Q15" s="2" t="n">
         <v>0.00155892745790896</v>
@@ -1254,6 +1342,12 @@
         <v>0.00155892745790896</v>
       </c>
       <c r="S15" s="2" t="n">
+        <v>0.00155892745790896</v>
+      </c>
+      <c r="T15" s="2" t="n">
+        <v>0.00155892745790896</v>
+      </c>
+      <c r="U15" s="2" t="n">
         <v>0.00160068295806211</v>
       </c>
     </row>
@@ -1285,20 +1379,20 @@
       <c r="J16" t="n">
         <v>14</v>
       </c>
-      <c r="L16" s="2" t="n">
-        <v>0.00135440180586907</v>
+      <c r="K16" t="n">
+        <v>14</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>0.00135424895609976</v>
+        <v>0.00135470760894107</v>
       </c>
       <c r="N16" s="2" t="n">
+        <v>0.00135455469014561</v>
+      </c>
+      <c r="O16" s="2" t="n">
         <v>0.00231481481481481</v>
       </c>
-      <c r="O16" s="2" t="n">
+      <c r="P16" s="2" t="n">
         <v>0.00149397076085797</v>
-      </c>
-      <c r="P16" s="2" t="n">
-        <v>0.00145499896071503</v>
       </c>
       <c r="Q16" s="2" t="n">
         <v>0.00145499896071503</v>
@@ -1307,6 +1401,12 @@
         <v>0.00145499896071503</v>
       </c>
       <c r="S16" s="2" t="n">
+        <v>0.00145499896071503</v>
+      </c>
+      <c r="T16" s="2" t="n">
+        <v>0.00145499896071503</v>
+      </c>
+      <c r="U16" s="2" t="n">
         <v>0.00149397076085797</v>
       </c>
     </row>
@@ -1336,22 +1436,22 @@
         <v>13</v>
       </c>
       <c r="J17" t="n">
+        <v>13</v>
+      </c>
+      <c r="K17" t="n">
         <v>12</v>
       </c>
-      <c r="L17" s="2" t="n">
-        <v>0.00124153498871332</v>
-      </c>
       <c r="M17" s="2" t="n">
-        <v>0.00124139487642478</v>
+        <v>0.00124181530819598</v>
       </c>
       <c r="N17" s="2" t="n">
+        <v>0.00124167513263348</v>
+      </c>
+      <c r="O17" s="2" t="n">
         <v>0.00462962962962963</v>
       </c>
-      <c r="O17" s="2" t="n">
+      <c r="P17" s="2" t="n">
         <v>0.00128054636644969</v>
-      </c>
-      <c r="P17" s="2" t="n">
-        <v>0.0013510704635211</v>
       </c>
       <c r="Q17" s="2" t="n">
         <v>0.0013510704635211</v>
@@ -1360,15 +1460,21 @@
         <v>0.0013510704635211</v>
       </c>
       <c r="S17" s="2" t="n">
+        <v>0.0013510704635211</v>
+      </c>
+      <c r="T17" s="2" t="n">
+        <v>0.0013510704635211</v>
+      </c>
+      <c r="U17" s="2" t="n">
         <v>0.00128054636644969</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:J17">
+  <conditionalFormatting sqref="C3:K17">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
-        <cfvo type="num" val="158.5"/>
+        <cfvo type="num" val="160"/>
         <cfvo type="num" val="2388"/>
         <color rgb="FFABDDA4"/>
         <color rgb="FFFFFFBF"/>
@@ -1376,12 +1482,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:S17">
+  <conditionalFormatting sqref="M3:U17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.0177142247358873"/>
-        <cfvo type="num" val="0.25744920993228"/>
+        <cfvo type="num" val="0.257507337999548"/>
         <color rgb="FFABDDA4"/>
         <color rgb="FFFFFFBF"/>
         <color rgb="FFFDAE61"/>
@@ -1438,29 +1544,35 @@
       <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2">
@@ -1490,12 +1602,12 @@
         <v>4912</v>
       </c>
       <c r="J2" s="1" t="n">
+        <v>4912</v>
+      </c>
+      <c r="K2" s="1" t="n">
         <v>4848</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="L2" s="1"/>
       <c r="M2" s="1" t="n">
         <v>1</v>
       </c>
@@ -1517,18 +1629,25 @@
       <c r="S2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
+      <c r="T2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" t="n">
         <v>1960</v>
@@ -1552,22 +1671,22 @@
         <v>2113</v>
       </c>
       <c r="J3" t="n">
+        <v>2113</v>
+      </c>
+      <c r="K3" t="n">
         <v>2073</v>
       </c>
-      <c r="L3" s="2" t="n">
+      <c r="M3" s="2" t="n">
         <v>0.423052018130801</v>
       </c>
-      <c r="M3" s="2" t="n">
+      <c r="N3" s="2" t="n">
         <v>0.423783783783784</v>
       </c>
-      <c r="N3" s="2" t="n">
+      <c r="O3" s="2" t="n">
         <v>0.674657534246575</v>
       </c>
-      <c r="O3" s="2" t="n">
+      <c r="P3" s="2" t="n">
         <v>0.42759900990099</v>
-      </c>
-      <c r="P3" s="2" t="n">
-        <v>0.430171009771987</v>
       </c>
       <c r="Q3" s="2" t="n">
         <v>0.430171009771987</v>
@@ -1576,6 +1695,12 @@
         <v>0.430171009771987</v>
       </c>
       <c r="S3" s="2" t="n">
+        <v>0.430171009771987</v>
+      </c>
+      <c r="T3" s="2" t="n">
+        <v>0.430171009771987</v>
+      </c>
+      <c r="U3" s="2" t="n">
         <v>0.42759900990099</v>
       </c>
     </row>
@@ -1605,22 +1730,22 @@
         <v>1570</v>
       </c>
       <c r="J4" t="n">
+        <v>1570</v>
+      </c>
+      <c r="K4" t="n">
         <v>1556</v>
       </c>
-      <c r="L4" s="2" t="n">
+      <c r="M4" s="2" t="n">
         <v>0.322037556658752</v>
       </c>
-      <c r="M4" s="2" t="n">
+      <c r="N4" s="2" t="n">
         <v>0.322594594594595</v>
       </c>
-      <c r="N4" s="2" t="n">
-        <v>0</v>
-      </c>
       <c r="O4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2" t="n">
         <v>0.320957095709571</v>
-      </c>
-      <c r="P4" s="2" t="n">
-        <v>0.319625407166124</v>
       </c>
       <c r="Q4" s="2" t="n">
         <v>0.319625407166124</v>
@@ -1629,6 +1754,12 @@
         <v>0.319625407166124</v>
       </c>
       <c r="S4" s="2" t="n">
+        <v>0.319625407166124</v>
+      </c>
+      <c r="T4" s="2" t="n">
+        <v>0.319625407166124</v>
+      </c>
+      <c r="U4" s="2" t="n">
         <v>0.320957095709571</v>
       </c>
     </row>
@@ -1658,22 +1789,22 @@
         <v>644</v>
       </c>
       <c r="J5" t="n">
+        <v>644</v>
+      </c>
+      <c r="K5" t="n">
         <v>640</v>
       </c>
-      <c r="L5" s="2" t="n">
+      <c r="M5" s="2" t="n">
         <v>0.132743362831858</v>
       </c>
-      <c r="M5" s="2" t="n">
+      <c r="N5" s="2" t="n">
         <v>0.132972972972973</v>
       </c>
-      <c r="N5" s="2" t="n">
+      <c r="O5" s="2" t="n">
         <v>0.182648401826484</v>
       </c>
-      <c r="O5" s="2" t="n">
+      <c r="P5" s="2" t="n">
         <v>0.132013201320132</v>
-      </c>
-      <c r="P5" s="2" t="n">
-        <v>0.131107491856678</v>
       </c>
       <c r="Q5" s="2" t="n">
         <v>0.131107491856678</v>
@@ -1682,6 +1813,12 @@
         <v>0.131107491856678</v>
       </c>
       <c r="S5" s="2" t="n">
+        <v>0.131107491856678</v>
+      </c>
+      <c r="T5" s="2" t="n">
+        <v>0.131107491856678</v>
+      </c>
+      <c r="U5" s="2" t="n">
         <v>0.132013201320132</v>
       </c>
     </row>
@@ -1711,22 +1848,22 @@
         <v>184</v>
       </c>
       <c r="J6" t="n">
+        <v>184</v>
+      </c>
+      <c r="K6" t="n">
         <v>182</v>
       </c>
-      <c r="L6" s="2" t="n">
+      <c r="M6" s="2" t="n">
         <v>0.0379883444852148</v>
       </c>
-      <c r="M6" s="2" t="n">
+      <c r="N6" s="2" t="n">
         <v>0.0380540540540541</v>
       </c>
-      <c r="N6" s="2" t="n">
+      <c r="O6" s="2" t="n">
         <v>0.0593607305936073</v>
       </c>
-      <c r="O6" s="2" t="n">
+      <c r="P6" s="2" t="n">
         <v>0.0375412541254125</v>
-      </c>
-      <c r="P6" s="2" t="n">
-        <v>0.0374592833876222</v>
       </c>
       <c r="Q6" s="2" t="n">
         <v>0.0374592833876222</v>
@@ -1735,6 +1872,12 @@
         <v>0.0374592833876222</v>
       </c>
       <c r="S6" s="2" t="n">
+        <v>0.0374592833876222</v>
+      </c>
+      <c r="T6" s="2" t="n">
+        <v>0.0374592833876222</v>
+      </c>
+      <c r="U6" s="2" t="n">
         <v>0.0375412541254125</v>
       </c>
     </row>
@@ -1764,22 +1907,22 @@
         <v>171</v>
       </c>
       <c r="J7" t="n">
+        <v>171</v>
+      </c>
+      <c r="K7" t="n">
         <v>169</v>
       </c>
-      <c r="L7" s="2" t="n">
+      <c r="M7" s="2" t="n">
         <v>0.0351823872221023</v>
       </c>
-      <c r="M7" s="2" t="n">
+      <c r="N7" s="2" t="n">
         <v>0.0352432432432432</v>
       </c>
-      <c r="N7" s="2" t="n">
+      <c r="O7" s="2" t="n">
         <v>0.0490867579908676</v>
       </c>
-      <c r="O7" s="2" t="n">
+      <c r="P7" s="2" t="n">
         <v>0.0348597359735974</v>
-      </c>
-      <c r="P7" s="2" t="n">
-        <v>0.0348127035830619</v>
       </c>
       <c r="Q7" s="2" t="n">
         <v>0.0348127035830619</v>
@@ -1788,6 +1931,12 @@
         <v>0.0348127035830619</v>
       </c>
       <c r="S7" s="2" t="n">
+        <v>0.0348127035830619</v>
+      </c>
+      <c r="T7" s="2" t="n">
+        <v>0.0348127035830619</v>
+      </c>
+      <c r="U7" s="2" t="n">
         <v>0.0348597359735974</v>
       </c>
     </row>
@@ -1817,22 +1966,22 @@
         <v>139</v>
       </c>
       <c r="J8" t="n">
+        <v>139</v>
+      </c>
+      <c r="K8" t="n">
         <v>137</v>
       </c>
-      <c r="L8" s="2" t="n">
+      <c r="M8" s="2" t="n">
         <v>0.0289229440966976</v>
       </c>
-      <c r="M8" s="2" t="n">
+      <c r="N8" s="2" t="n">
         <v>0.028972972972973</v>
       </c>
-      <c r="N8" s="2" t="n">
+      <c r="O8" s="2" t="n">
         <v>0.0182648401826484</v>
       </c>
-      <c r="O8" s="2" t="n">
+      <c r="P8" s="2" t="n">
         <v>0.0282590759075908</v>
-      </c>
-      <c r="P8" s="2" t="n">
-        <v>0.0282980456026059</v>
       </c>
       <c r="Q8" s="2" t="n">
         <v>0.0282980456026059</v>
@@ -1841,6 +1990,12 @@
         <v>0.0282980456026059</v>
       </c>
       <c r="S8" s="2" t="n">
+        <v>0.0282980456026059</v>
+      </c>
+      <c r="T8" s="2" t="n">
+        <v>0.0282980456026059</v>
+      </c>
+      <c r="U8" s="2" t="n">
         <v>0.0282590759075908</v>
       </c>
     </row>
@@ -1872,20 +2027,20 @@
       <c r="J9" t="n">
         <v>49</v>
       </c>
-      <c r="L9" s="2" t="n">
+      <c r="K9" t="n">
+        <v>49</v>
+      </c>
+      <c r="M9" s="2" t="n">
         <v>0.0103604575868768</v>
       </c>
-      <c r="M9" s="2" t="n">
+      <c r="N9" s="2" t="n">
         <v>0.0103783783783784</v>
       </c>
-      <c r="N9" s="2" t="n">
+      <c r="O9" s="2" t="n">
         <v>0.0045662100456621</v>
       </c>
-      <c r="O9" s="2" t="n">
+      <c r="P9" s="2" t="n">
         <v>0.0101072607260726</v>
-      </c>
-      <c r="P9" s="2" t="n">
-        <v>0.00997557003257329</v>
       </c>
       <c r="Q9" s="2" t="n">
         <v>0.00997557003257329</v>
@@ -1894,6 +2049,12 @@
         <v>0.00997557003257329</v>
       </c>
       <c r="S9" s="2" t="n">
+        <v>0.00997557003257329</v>
+      </c>
+      <c r="T9" s="2" t="n">
+        <v>0.00997557003257329</v>
+      </c>
+      <c r="U9" s="2" t="n">
         <v>0.0101072607260726</v>
       </c>
     </row>
@@ -1925,20 +2086,20 @@
       <c r="J10" t="n">
         <v>27</v>
       </c>
-      <c r="L10" s="2" t="n">
+      <c r="K10" t="n">
+        <v>27</v>
+      </c>
+      <c r="M10" s="2" t="n">
         <v>0.00496438592704511</v>
       </c>
-      <c r="M10" s="2" t="n">
+      <c r="N10" s="2" t="n">
         <v>0.00497297297297297</v>
       </c>
-      <c r="N10" s="2" t="n">
+      <c r="O10" s="2" t="n">
         <v>0.00799086757990868</v>
       </c>
-      <c r="O10" s="2" t="n">
+      <c r="P10" s="2" t="n">
         <v>0.00556930693069307</v>
-      </c>
-      <c r="P10" s="2" t="n">
-        <v>0.00549674267100977</v>
       </c>
       <c r="Q10" s="2" t="n">
         <v>0.00549674267100977</v>
@@ -1947,12 +2108,18 @@
         <v>0.00549674267100977</v>
       </c>
       <c r="S10" s="2" t="n">
+        <v>0.00549674267100977</v>
+      </c>
+      <c r="T10" s="2" t="n">
+        <v>0.00549674267100977</v>
+      </c>
+      <c r="U10" s="2" t="n">
         <v>0.00556930693069307</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" t="n">
         <v>14</v>
@@ -1978,20 +2145,20 @@
       <c r="J11" t="n">
         <v>15</v>
       </c>
-      <c r="L11" s="2" t="n">
+      <c r="K11" t="n">
+        <v>15</v>
+      </c>
+      <c r="M11" s="2" t="n">
         <v>0.00302180012950572</v>
       </c>
-      <c r="M11" s="2" t="n">
+      <c r="N11" s="2" t="n">
         <v>0.00302702702702703</v>
       </c>
-      <c r="N11" s="2" t="n">
+      <c r="O11" s="2" t="n">
         <v>0.00342465753424658</v>
       </c>
-      <c r="O11" s="2" t="n">
+      <c r="P11" s="2" t="n">
         <v>0.00309405940594059</v>
-      </c>
-      <c r="P11" s="2" t="n">
-        <v>0.00305374592833876</v>
       </c>
       <c r="Q11" s="2" t="n">
         <v>0.00305374592833876</v>
@@ -2000,12 +2167,18 @@
         <v>0.00305374592833876</v>
       </c>
       <c r="S11" s="2" t="n">
+        <v>0.00305374592833876</v>
+      </c>
+      <c r="T11" s="2" t="n">
+        <v>0.00305374592833876</v>
+      </c>
+      <c r="U11" s="2" t="n">
         <v>0.00309405940594059</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" t="n">
         <v>8</v>
@@ -2031,12 +2204,12 @@
       <c r="J12" t="n">
         <v>0</v>
       </c>
-      <c r="L12" s="2" t="n">
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2" t="n">
         <v>0.00172674293114613</v>
       </c>
-      <c r="M12" s="2" t="n">
-        <v>0</v>
-      </c>
       <c r="N12" s="2" t="n">
         <v>0</v>
       </c>
@@ -2055,13 +2228,19 @@
       <c r="S12" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="T12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:J12">
+  <conditionalFormatting sqref="C3:K12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
-        <cfvo type="num" val="138"/>
+        <cfvo type="num" val="139"/>
         <cfvo type="num" val="2113"/>
         <color rgb="FFABDDA4"/>
         <color rgb="FFFFFFBF"/>
@@ -2069,7 +2248,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:S12">
+  <conditionalFormatting sqref="M3:U12">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Re-run mock data analysis
Differences in the QIIME2 and Amptk pipelines are due to
changes in primer handling (different consensus method
for primer mixes). Besides, Amptk always generates slightly different
results at every run (not sure why).
</commit_message>
<xml_diff>
--- a/test/cmp/ITS__ITS3-KYO2...ITS4.xlsx
+++ b/test/cmp/ITS__ITS3-KYO2...ITS4.xlsx
@@ -511,13 +511,13 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="n">
-        <v>8864</v>
+        <v>8928</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>8864</v>
+        <v>8928</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>1726</v>
+        <v>1728</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>9371</v>
@@ -573,10 +573,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>2283</v>
+        <v>2282</v>
       </c>
       <c r="D3" t="n">
-        <v>2283</v>
+        <v>2282</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -597,10 +597,10 @@
         <v>2366</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>0.257558664259928</v>
+        <v>0.255600358422939</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>0.257558664259928</v>
+        <v>0.255600358422939</v>
       </c>
       <c r="N3" s="2" t="n">
         <v>0</v>
@@ -626,13 +626,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="D4" t="n">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="E4" t="n">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F4" t="n">
         <v>1561</v>
@@ -650,13 +650,13 @@
         <v>1561</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>0.170803249097473</v>
+        <v>0.169354838709677</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>0.170803249097473</v>
+        <v>0.169354838709677</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>0.249710312862109</v>
+        <v>0.248842592592593</v>
       </c>
       <c r="O4" s="2" t="n">
         <v>0.166577739835663</v>
@@ -679,10 +679,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D5" t="n">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="E5" t="n">
         <v>343</v>
@@ -703,13 +703,13 @@
         <v>1276</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>0.139101985559567</v>
+        <v>0.138216845878136</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>0.139101985559567</v>
+        <v>0.138216845878136</v>
       </c>
       <c r="N5" s="2" t="n">
-        <v>0.198725376593279</v>
+        <v>0.19849537037037</v>
       </c>
       <c r="O5" s="2" t="n">
         <v>0.136164763632483</v>
@@ -732,10 +732,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="D6" t="n">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="E6" t="n">
         <v>160</v>
@@ -756,13 +756,13 @@
         <v>1177</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>0.128497292418773</v>
+        <v>0.127352150537634</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>0.128497292418773</v>
+        <v>0.127352150537634</v>
       </c>
       <c r="N6" s="2" t="n">
-        <v>0.0926998841251448</v>
+        <v>0.0925925925925926</v>
       </c>
       <c r="O6" s="2" t="n">
         <v>0.125600256109273</v>
@@ -791,7 +791,7 @@
         <v>931</v>
       </c>
       <c r="E7" t="n">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F7" t="n">
         <v>979</v>
@@ -809,13 +809,13 @@
         <v>979</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>0.105031588447653</v>
+        <v>0.104278673835125</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>0.105031588447653</v>
+        <v>0.104278673835125</v>
       </c>
       <c r="N7" s="2" t="n">
-        <v>0.149478563151796</v>
+        <v>0.149884259259259</v>
       </c>
       <c r="O7" s="2" t="n">
         <v>0.104471241062853</v>
@@ -838,10 +838,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>808</v>
+        <v>875</v>
       </c>
       <c r="D8" t="n">
-        <v>808</v>
+        <v>875</v>
       </c>
       <c r="E8" t="n">
         <v>223</v>
@@ -862,13 +862,13 @@
         <v>929</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>0.0911552346570397</v>
+        <v>0.0980062724014337</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>0.0911552346570397</v>
+        <v>0.0980062724014337</v>
       </c>
       <c r="N8" s="2" t="n">
-        <v>0.129200463499421</v>
+        <v>0.129050925925926</v>
       </c>
       <c r="O8" s="2" t="n">
         <v>0.0991356312026465</v>
@@ -897,7 +897,7 @@
         <v>515</v>
       </c>
       <c r="E9" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F9" t="n">
         <v>621</v>
@@ -915,13 +915,13 @@
         <v>621</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>0.0581001805054152</v>
+        <v>0.0576836917562724</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>0.0581001805054152</v>
+        <v>0.0576836917562724</v>
       </c>
       <c r="N9" s="2" t="n">
-        <v>0.115295480880649</v>
+        <v>0.115740740740741</v>
       </c>
       <c r="O9" s="2" t="n">
         <v>0.0662682744637712</v>
@@ -944,10 +944,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D10" t="n">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E10" t="n">
         <v>42</v>
@@ -968,13 +968,13 @@
         <v>166</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>0.0178249097472924</v>
+        <v>0.0175851254480287</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>0.0178249097472924</v>
+        <v>0.0175851254480287</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>0.0243337195828505</v>
+        <v>0.0243055555555556</v>
       </c>
       <c r="O10" s="2" t="n">
         <v>0.0177142247358873</v>
@@ -1021,13 +1021,13 @@
         <v>98</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>0.0107175090252708</v>
+        <v>0.0106406810035842</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>0.0107175090252708</v>
+        <v>0.0106406810035842</v>
       </c>
       <c r="N11" s="2" t="n">
-        <v>0.0208574739281576</v>
+        <v>0.0208333333333333</v>
       </c>
       <c r="O11" s="2" t="n">
         <v>0.0104577953260058</v>
@@ -1074,10 +1074,10 @@
         <v>95</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>0.0106046931407942</v>
+        <v>0.0105286738351254</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>0.0106046931407942</v>
+        <v>0.0105286738351254</v>
       </c>
       <c r="N12" s="2" t="n">
         <v>0</v>
@@ -1127,13 +1127,13 @@
         <v>38</v>
       </c>
       <c r="L13" s="2" t="n">
-        <v>0.0039485559566787</v>
+        <v>0.00392025089605735</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>0.0039485559566787</v>
+        <v>0.00392025089605735</v>
       </c>
       <c r="N13" s="2" t="n">
-        <v>0.00869061413673233</v>
+        <v>0.00868055555555556</v>
       </c>
       <c r="O13" s="2" t="n">
         <v>0.00405506349375734</v>
@@ -1180,10 +1180,10 @@
         <v>24</v>
       </c>
       <c r="L14" s="2" t="n">
-        <v>0.00259476534296029</v>
+        <v>0.00257616487455197</v>
       </c>
       <c r="M14" s="2" t="n">
-        <v>0.00259476534296029</v>
+        <v>0.00257616487455197</v>
       </c>
       <c r="N14" s="2" t="n">
         <v>0</v>
@@ -1209,10 +1209,10 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E15" t="n">
         <v>7</v>
@@ -1233,13 +1233,13 @@
         <v>15</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>0.00146660649819495</v>
+        <v>0.00156810035842294</v>
       </c>
       <c r="M15" s="2" t="n">
-        <v>0.00146660649819495</v>
+        <v>0.00156810035842294</v>
       </c>
       <c r="N15" s="2" t="n">
-        <v>0.00405561993047509</v>
+        <v>0.00405092592592593</v>
       </c>
       <c r="O15" s="2" t="n">
         <v>0.00160068295806211</v>
@@ -1262,10 +1262,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" t="n">
         <v>4</v>
@@ -1286,13 +1286,13 @@
         <v>14</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>0.00135379061371841</v>
+        <v>0.00145609318996416</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>0.00135379061371841</v>
+        <v>0.00145609318996416</v>
       </c>
       <c r="N16" s="2" t="n">
-        <v>0.00231749710312862</v>
+        <v>0.00231481481481481</v>
       </c>
       <c r="O16" s="2" t="n">
         <v>0.00149397076085797</v>
@@ -1321,7 +1321,7 @@
         <v>11</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>12</v>
@@ -1339,13 +1339,13 @@
         <v>12</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>0.00124097472924188</v>
+        <v>0.00123207885304659</v>
       </c>
       <c r="M17" s="2" t="n">
-        <v>0.00124097472924188</v>
+        <v>0.00123207885304659</v>
       </c>
       <c r="N17" s="2" t="n">
-        <v>0.00463499420625724</v>
+        <v>0.00520833333333333</v>
       </c>
       <c r="O17" s="2" t="n">
         <v>0.00128054636644969</v>
@@ -1368,7 +1368,7 @@
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
-        <cfvo type="num" val="159"/>
+        <cfvo type="num" val="158.5"/>
         <cfvo type="num" val="2388"/>
         <color rgb="FFABDDA4"/>
         <color rgb="FFFFFFBF"/>
@@ -1380,8 +1380,8 @@
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.0177142247358873"/>
-        <cfvo type="num" val="0.257558664259928"/>
+        <cfvo type="num" val="0.0175851254480287"/>
+        <cfvo type="num" val="0.255600358422939"/>
         <color rgb="FFABDDA4"/>
         <color rgb="FFFFFFBF"/>
         <color rgb="FFFDAE61"/>
@@ -1469,13 +1469,13 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="n">
-        <v>4638</v>
+        <v>4632</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>4630</v>
+        <v>4624</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>4848</v>
@@ -1531,10 +1531,10 @@
         <v>26</v>
       </c>
       <c r="C3" t="n">
-        <v>1961</v>
+        <v>1958</v>
       </c>
       <c r="D3" t="n">
-        <v>1961</v>
+        <v>1958</v>
       </c>
       <c r="E3" t="n">
         <v>591</v>
@@ -1555,13 +1555,13 @@
         <v>2073</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>0.422811556705476</v>
+        <v>0.422711571675302</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>0.42354211663067</v>
+        <v>0.423442906574394</v>
       </c>
       <c r="N3" s="2" t="n">
-        <v>0.673888255416192</v>
+        <v>0.675428571428571</v>
       </c>
       <c r="O3" s="2" t="n">
         <v>0.42759900990099</v>
@@ -1584,10 +1584,10 @@
         <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="D4" t="n">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -1608,10 +1608,10 @@
         <v>1556</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>0.322121604139715</v>
+        <v>0.322107081174439</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>0.32267818574514</v>
+        <v>0.322664359861592</v>
       </c>
       <c r="N4" s="2" t="n">
         <v>0</v>
@@ -1637,10 +1637,10 @@
         <v>16</v>
       </c>
       <c r="C5" t="n">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="D5" t="n">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E5" t="n">
         <v>160</v>
@@ -1661,13 +1661,13 @@
         <v>640</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>0.133031479085813</v>
+        <v>0.132556131260794</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>0.133261339092873</v>
+        <v>0.132785467128028</v>
       </c>
       <c r="N5" s="2" t="n">
-        <v>0.182440136830103</v>
+        <v>0.182857142857143</v>
       </c>
       <c r="O5" s="2" t="n">
         <v>0.132013201320132</v>
@@ -1714,13 +1714,13 @@
         <v>182</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>0.0379473911168607</v>
+        <v>0.0379965457685665</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>0.0380129589632829</v>
+        <v>0.0380622837370242</v>
       </c>
       <c r="N6" s="2" t="n">
-        <v>0.0592930444697834</v>
+        <v>0.0594285714285714</v>
       </c>
       <c r="O6" s="2" t="n">
         <v>0.0375412541254125</v>
@@ -1743,13 +1743,13 @@
         <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D7" t="n">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E7" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F7" t="n">
         <v>169</v>
@@ -1767,13 +1767,13 @@
         <v>169</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>0.0351444588184562</v>
+        <v>0.0349740932642487</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>0.0352051835853132</v>
+        <v>0.0350346020761246</v>
       </c>
       <c r="N7" s="2" t="n">
-        <v>0.0501710376282782</v>
+        <v>0.048</v>
       </c>
       <c r="O7" s="2" t="n">
         <v>0.0348597359735974</v>
@@ -1796,10 +1796,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D8" t="n">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E8" t="n">
         <v>16</v>
@@ -1820,13 +1820,13 @@
         <v>137</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>0.0288917636912462</v>
+        <v>0.0291450777202073</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>0.0289416846652268</v>
+        <v>0.0291955017301038</v>
       </c>
       <c r="N8" s="2" t="n">
-        <v>0.0182440136830103</v>
+        <v>0.0182857142857143</v>
       </c>
       <c r="O8" s="2" t="n">
         <v>0.0282590759075908</v>
@@ -1873,13 +1873,13 @@
         <v>49</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>0.0103492884864166</v>
+        <v>0.0103626943005181</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>0.0103671706263499</v>
+        <v>0.0103806228373702</v>
       </c>
       <c r="N9" s="2" t="n">
-        <v>0.00456100342075257</v>
+        <v>0.00457142857142857</v>
       </c>
       <c r="O9" s="2" t="n">
         <v>0.0101072607260726</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="C10" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D10" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E10" t="n">
         <v>7</v>
@@ -1926,13 +1926,13 @@
         <v>27</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>0.00495903406640793</v>
+        <v>0.00539723661485319</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>0.00496760259179266</v>
+        <v>0.00540657439446367</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>0.00798175598631699</v>
+        <v>0.008</v>
       </c>
       <c r="O10" s="2" t="n">
         <v>0.00556930693069307</v>
@@ -1979,13 +1979,13 @@
         <v>15</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>0.00301854247520483</v>
+        <v>0.00302245250431779</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>0.00302375809935205</v>
+        <v>0.00302768166089965</v>
       </c>
       <c r="N11" s="2" t="n">
-        <v>0.00342075256556442</v>
+        <v>0.00342857142857143</v>
       </c>
       <c r="O11" s="2" t="n">
         <v>0.00309405940594059</v>
@@ -2032,7 +2032,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>0.00172488141440276</v>
+        <v>0.00172711571675302</v>
       </c>
       <c r="M12" s="2" t="n">
         <v>0</v>
@@ -2073,8 +2073,8 @@
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.0289167241782365"/>
-        <cfvo type="num" val="0.673888255416192"/>
+        <cfvo type="num" val="0.0291702897251555"/>
+        <cfvo type="num" val="0.675428571428571"/>
         <color rgb="FFABDDA4"/>
         <color rgb="FFFFFFBF"/>
         <color rgb="FFFDAE61"/>

</xml_diff>